<commit_message>
Actualización de contraseña de equipos de monitoreo
Actualizada la contraseña del usuario "DTO Monitoreo" de las unidades de
monitoreo 1 y 2.
</commit_message>
<xml_diff>
--- a/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
+++ b/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="394" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="394"/>
   </bookViews>
   <sheets>
     <sheet name="Servidor" sheetId="1" r:id="rId1"/>
@@ -556,9 +556,6 @@
     <t>Administracion / DTO Monitoreo</t>
   </si>
   <si>
-    <t>hola1234 / cck123</t>
-  </si>
-  <si>
     <t>Intel i3 / 4 Gb mem</t>
   </si>
   <si>
@@ -665,6 +662,9 @@
   </si>
   <si>
     <t>W_Gomez</t>
+  </si>
+  <si>
+    <t>hola1234 / 12345678</t>
   </si>
 </sst>
 </file>
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1194,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
@@ -1301,13 +1301,13 @@
         <v>177</v>
       </c>
       <c r="F4" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="G4" t="s">
         <v>122</v>
       </c>
       <c r="J4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1324,13 +1324,13 @@
         <v>177</v>
       </c>
       <c r="F5" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="G5" t="s">
         <v>122</v>
       </c>
       <c r="J5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1475,7 @@
         <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
         <v>73</v>
       </c>
       <c r="J8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1587,10 +1587,10 @@
         <v>5432</v>
       </c>
       <c r="E9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H9" t="s">
         <v>186</v>
-      </c>
-      <c r="H9" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1635,25 +1635,25 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
         <v>181</v>
-      </c>
-      <c r="B12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C12" t="s">
-        <v>182</v>
       </c>
       <c r="D12">
         <v>1433</v>
       </c>
       <c r="E12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" t="s">
         <v>183</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>184</v>
-      </c>
-      <c r="H12" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1670,7 +1670,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1890,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,7 +2574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -2602,10 +2602,10 @@
         <v>83</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2622,10 +2622,10 @@
         <v>89</v>
       </c>
       <c r="E2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" t="s">
         <v>196</v>
-      </c>
-      <c r="F2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2662,10 +2662,10 @@
         <v>90</v>
       </c>
       <c r="E4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" t="s">
         <v>198</v>
-      </c>
-      <c r="F4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2682,10 +2682,10 @@
         <v>91</v>
       </c>
       <c r="E5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" t="s">
         <v>200</v>
-      </c>
-      <c r="F5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2702,10 +2702,10 @@
         <v>92</v>
       </c>
       <c r="E6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" t="s">
         <v>202</v>
-      </c>
-      <c r="F6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2719,10 +2719,10 @@
         <v>93</v>
       </c>
       <c r="E7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" t="s">
         <v>204</v>
-      </c>
-      <c r="F7" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2733,10 +2733,10 @@
         <v>94</v>
       </c>
       <c r="E8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" t="s">
         <v>206</v>
-      </c>
-      <c r="F8" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2747,10 +2747,10 @@
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2761,10 +2761,10 @@
         <v>96</v>
       </c>
       <c r="E10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" t="s">
         <v>209</v>
-      </c>
-      <c r="F10" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,10 +2775,10 @@
         <v>97</v>
       </c>
       <c r="E11" t="s">
+        <v>210</v>
+      </c>
+      <c r="F11" t="s">
         <v>211</v>
-      </c>
-      <c r="F11" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2789,10 +2789,10 @@
         <v>98</v>
       </c>
       <c r="E12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F12" t="s">
         <v>213</v>
-      </c>
-      <c r="F12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,32 +2946,32 @@
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregada lista de banderas
Agregada una planilla con la lista de banderas configuradas en la
iluminación de la cúpula.
</commit_message>
<xml_diff>
--- a/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
+++ b/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="394"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="394" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Servidor" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Alias" sheetId="5" r:id="rId5"/>
     <sheet name="Sistemas" sheetId="6" r:id="rId6"/>
     <sheet name="Usuarios" sheetId="7" r:id="rId7"/>
+    <sheet name="Panel de banderas" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="234">
   <si>
     <t>Servidor</t>
   </si>
@@ -665,13 +666,70 @@
   </si>
   <si>
     <t>hola1234 / 12345678</t>
+  </si>
+  <si>
+    <t>1 Argentina</t>
+  </si>
+  <si>
+    <t>2 Show Argentina</t>
+  </si>
+  <si>
+    <t>3 Brasil</t>
+  </si>
+  <si>
+    <t>4 Chile</t>
+  </si>
+  <si>
+    <t>5 Show Latinoamérica</t>
+  </si>
+  <si>
+    <t>6 Uruguay</t>
+  </si>
+  <si>
+    <t>7 Paraguay</t>
+  </si>
+  <si>
+    <t>8 Venezuela, Colombia, Ecuador</t>
+  </si>
+  <si>
+    <t>1 Bolivia</t>
+  </si>
+  <si>
+    <t>2 España</t>
+  </si>
+  <si>
+    <t>3 Italia</t>
+  </si>
+  <si>
+    <t>4 Francia</t>
+  </si>
+  <si>
+    <t>5 Show luces blancas</t>
+  </si>
+  <si>
+    <t>6 Magenta</t>
+  </si>
+  <si>
+    <t>7 Cian</t>
+  </si>
+  <si>
+    <t>8 Diversidad</t>
+  </si>
+  <si>
+    <t>Izquierda (panel 1)</t>
+  </si>
+  <si>
+    <t>Derecha (panel 2)</t>
+  </si>
+  <si>
+    <t>(*) Se apaga con el botón gris</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,6 +741,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -721,13 +787,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1183,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2981,4 +3048,101 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizada la planilla de sistemas
Se agregaron los sistemas que faltaban y los usuarios, contraseñas y
datos de acceso de las bases de datos faltantes.
</commit_message>
<xml_diff>
--- a/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
+++ b/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="394" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="394" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Servidor" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="282">
   <si>
     <t>Servidor</t>
   </si>
@@ -422,12 +422,6 @@
     <t>192.168.201.65</t>
   </si>
   <si>
-    <t>marce</t>
-  </si>
-  <si>
-    <t>Mastropiero!</t>
-  </si>
-  <si>
     <t>Adrián Acua 15-5716-6544</t>
   </si>
   <si>
@@ -729,6 +723,150 @@
   </si>
   <si>
     <t>!ministerio16</t>
+  </si>
+  <si>
+    <t>ameana</t>
+  </si>
+  <si>
+    <t>apellegrotti</t>
+  </si>
+  <si>
+    <t>controlaccesob</t>
+  </si>
+  <si>
+    <t>ctreser</t>
+  </si>
+  <si>
+    <t>ebaez</t>
+  </si>
+  <si>
+    <t>esapciosfisicos</t>
+  </si>
+  <si>
+    <t>evedoya</t>
+  </si>
+  <si>
+    <t>ezemahafud</t>
+  </si>
+  <si>
+    <t>glotz</t>
+  </si>
+  <si>
+    <t>hacosta</t>
+  </si>
+  <si>
+    <t>hgoni</t>
+  </si>
+  <si>
+    <t>limpieza</t>
+  </si>
+  <si>
+    <t>llavero</t>
+  </si>
+  <si>
+    <t>mchemes</t>
+  </si>
+  <si>
+    <t>mmarcote</t>
+  </si>
+  <si>
+    <t>mriccitelli</t>
+  </si>
+  <si>
+    <t>mrojas</t>
+  </si>
+  <si>
+    <t>nachog</t>
+  </si>
+  <si>
+    <t>nadiav</t>
+  </si>
+  <si>
+    <t>ngonzalez</t>
+  </si>
+  <si>
+    <t>rciccotosto</t>
+  </si>
+  <si>
+    <t>rlirusso</t>
+  </si>
+  <si>
+    <t>serviciosgenerales</t>
+  </si>
+  <si>
+    <t>sgutierre</t>
+  </si>
+  <si>
+    <t>vdevinco</t>
+  </si>
+  <si>
+    <t>Actualmente ya no se encuentra esta configuración en la panelera (16/09/16).</t>
+  </si>
+  <si>
+    <t>Servidor nuevo</t>
+  </si>
+  <si>
+    <t>10.13.19.178</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>Ss11!</t>
+  </si>
+  <si>
+    <t>Intel Xeon E5 / 6Gb mem / 500 Gb disco</t>
+  </si>
+  <si>
+    <t>CCKCyP2016!</t>
+  </si>
+  <si>
+    <t>ID TView: 788011903</t>
+  </si>
+  <si>
+    <t>Alarma de incendio y monitoreo de sensores</t>
+  </si>
+  <si>
+    <t>FAS</t>
+  </si>
+  <si>
+    <t>Alarma de intrusión</t>
+  </si>
+  <si>
+    <t>Notifier</t>
+  </si>
+  <si>
+    <t>Alarma de incendio con descarga de CO2</t>
+  </si>
+  <si>
+    <t>Sistema de CCTV</t>
+  </si>
+  <si>
+    <t>SCCTV</t>
+  </si>
+  <si>
+    <t>Sistema de certificación de facturas</t>
+  </si>
+  <si>
+    <t>CERT</t>
+  </si>
+  <si>
+    <t>http://gestionactivos.cck.gob.ar/facturas/</t>
+  </si>
+  <si>
+    <t>facturas</t>
+  </si>
+  <si>
+    <t>Debe apuntar a la IP: 192.168.1.1 y máscara: 255.255.255.0</t>
+  </si>
+  <si>
+    <t>FACTURAS</t>
+  </si>
+  <si>
+    <t>CONVENIOS</t>
+  </si>
+  <si>
+    <t>convenios</t>
   </si>
 </sst>
 </file>
@@ -793,7 +931,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -801,6 +939,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -866,8 +1007,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="A1:J5" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:J5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="A1:J6" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:J6"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Servidor"/>
     <tableColumn id="2" name="Dirección IP"/>
@@ -885,8 +1026,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="A1:K12" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:K12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="A1:K14" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:K14"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Servidor"/>
     <tableColumn id="2" name="Dirección IP"/>
@@ -929,8 +1070,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:O20" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:O20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:O25" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:O25"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Sistema"/>
     <tableColumn id="2" name="Nombre"/>
@@ -953,8 +1094,11 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A1:F37" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla52" displayName="Tabla52" ref="A1:F62" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F62"/>
+  <sortState ref="A2:F70">
+    <sortCondition ref="C1"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Pentaho producción"/>
     <tableColumn id="2" name="Pentaho desarrollo"/>
@@ -1254,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,7 +1415,7 @@
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" customWidth="1"/>
+    <col min="10" max="10" width="35.5703125" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1362,48 +1506,68 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" t="s">
         <v>173</v>
-      </c>
-      <c r="B4" t="s">
-        <v>175</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G4" t="s">
         <v>122</v>
       </c>
       <c r="J4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" t="s">
         <v>174</v>
-      </c>
-      <c r="B5" t="s">
-        <v>176</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G5" t="s">
         <v>122</v>
       </c>
       <c r="J5" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" t="s">
+        <v>263</v>
+      </c>
+      <c r="J6" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -1417,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1596,7 @@
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="16.140625" customWidth="1"/>
@@ -1548,7 +1712,7 @@
         <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1643,7 +1807,7 @@
         <v>73</v>
       </c>
       <c r="J8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1660,10 +1824,10 @@
         <v>5432</v>
       </c>
       <c r="E9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1708,25 +1872,68 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>5432</v>
+      </c>
+      <c r="E12" t="s">
+        <v>279</v>
+      </c>
+      <c r="H12" t="s">
+        <v>277</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13">
+        <v>5432</v>
+      </c>
+      <c r="E13" t="s">
+        <v>280</v>
+      </c>
+      <c r="H13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14">
+        <v>1433</v>
+      </c>
+      <c r="E14" t="s">
         <v>180</v>
       </c>
-      <c r="B12" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="F14" t="s">
         <v>181</v>
       </c>
-      <c r="D12">
-        <v>1433</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="H14" t="s">
         <v>182</v>
-      </c>
-      <c r="F12" t="s">
-        <v>183</v>
-      </c>
-      <c r="H12" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1796,10 +2003,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
@@ -1969,32 +2176,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="36" customWidth="1"/>
+    <col min="8" max="8" width="37.85546875" customWidth="1"/>
     <col min="9" max="9" width="36.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
     <col min="13" max="13" width="30.5703125" customWidth="1"/>
     <col min="14" max="14" width="33.42578125" customWidth="1"/>
-    <col min="15" max="15" width="46.28515625" customWidth="1"/>
+    <col min="15" max="15" width="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -2002,7 +2209,7 @@
         <v>45</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>123</v>
@@ -2011,16 +2218,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>46</v>
@@ -2058,7 +2265,7 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
@@ -2102,7 +2309,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -2146,7 +2353,7 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -2190,7 +2397,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -2234,7 +2441,7 @@
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
@@ -2278,7 +2485,7 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -2322,7 +2529,7 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -2366,7 +2573,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F9" t="s">
         <v>25</v>
@@ -2410,7 +2617,7 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -2442,19 +2649,19 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F11" t="s">
         <v>126</v>
@@ -2466,36 +2673,36 @@
         <v>125</v>
       </c>
       <c r="I11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N11" t="s">
         <v>122</v>
       </c>
       <c r="O11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F12" t="s">
         <v>128</v>
@@ -2506,36 +2713,39 @@
       <c r="N12" t="s">
         <v>122</v>
       </c>
+      <c r="O12" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
         <v>126</v>
@@ -2544,29 +2754,29 @@
         <v>127</v>
       </c>
       <c r="H14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="N14" t="s">
         <v>122</v>
       </c>
       <c r="O14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s">
         <v>129</v>
@@ -2574,10 +2784,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="N17" t="s">
         <v>122</v>
@@ -2585,7 +2795,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B18" t="s">
         <v>130</v>
@@ -2593,7 +2803,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
         <v>124</v>
@@ -2604,6 +2814,9 @@
       <c r="D19" t="s">
         <v>131</v>
       </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
       <c r="H19" t="s">
         <v>132</v>
       </c>
@@ -2611,34 +2824,110 @@
         <v>124</v>
       </c>
       <c r="J19" t="s">
+        <v>266</v>
+      </c>
+      <c r="K19" t="s">
+        <v>265</v>
+      </c>
+      <c r="M19" t="s">
         <v>133</v>
       </c>
-      <c r="K19" t="s">
+      <c r="N19" t="s">
         <v>134</v>
       </c>
-      <c r="M19" t="s">
+      <c r="O19" t="s">
         <v>135</v>
-      </c>
-      <c r="N19" t="s">
-        <v>136</v>
-      </c>
-      <c r="O19" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H20" s="5"/>
       <c r="L20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="N20" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>267</v>
+      </c>
+      <c r="B21" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>271</v>
+      </c>
+      <c r="B23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>272</v>
+      </c>
+      <c r="B24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>274</v>
+      </c>
+      <c r="B25" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I25" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" t="s">
+        <v>277</v>
+      </c>
+      <c r="K25" t="s">
+        <v>277</v>
+      </c>
+      <c r="L25" t="s">
+        <v>120</v>
+      </c>
+      <c r="M25" t="s">
+        <v>64</v>
+      </c>
+      <c r="N25" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2646,21 +2935,22 @@
     <hyperlink ref="H8" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
     <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="H25" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="landscape" r:id="rId4"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,10 +2977,10 @@
         <v>83</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2707,10 +2997,10 @@
         <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2727,10 +3017,10 @@
         <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2747,10 +3037,10 @@
         <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2761,16 +3051,16 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>234</v>
       </c>
       <c r="D5" t="s">
         <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2781,16 +3071,16 @@
         <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
         <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2798,91 +3088,91 @@
         <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
         <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>94</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
         <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>96</v>
+        <v>236</v>
       </c>
       <c r="D10" t="s">
         <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>97</v>
+        <v>237</v>
       </c>
       <c r="D11" t="s">
         <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
         <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="D13" t="s">
         <v>99</v>
@@ -2890,7 +3180,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="D14" t="s">
         <v>100</v>
@@ -2898,7 +3188,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>101</v>
+        <v>240</v>
       </c>
       <c r="D15" t="s">
         <v>101</v>
@@ -2906,7 +3196,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
         <v>102</v>
@@ -2914,7 +3204,7 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>103</v>
+        <v>241</v>
       </c>
       <c r="D17" t="s">
         <v>103</v>
@@ -2922,7 +3212,7 @@
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>104</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
         <v>104</v>
@@ -2930,7 +3220,7 @@
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
         <v>105</v>
@@ -2938,7 +3228,7 @@
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
         <v>106</v>
@@ -2946,7 +3236,7 @@
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>107</v>
+        <v>189</v>
       </c>
       <c r="D21" t="s">
         <v>107</v>
@@ -2954,7 +3244,7 @@
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
         <v>108</v>
@@ -2962,7 +3252,7 @@
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
         <v>109</v>
@@ -2970,7 +3260,7 @@
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>110</v>
+        <v>242</v>
       </c>
       <c r="D24" t="s">
         <v>110</v>
@@ -2978,7 +3268,7 @@
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
         <v>111</v>
@@ -2986,7 +3276,7 @@
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>112</v>
+        <v>243</v>
       </c>
       <c r="D26" t="s">
         <v>112</v>
@@ -2994,7 +3284,7 @@
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>113</v>
+        <v>244</v>
       </c>
       <c r="D27" t="s">
         <v>113</v>
@@ -3002,7 +3292,7 @@
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
         <v>114</v>
@@ -3010,7 +3300,7 @@
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
         <v>115</v>
@@ -3018,7 +3308,7 @@
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
         <v>116</v>
@@ -3026,37 +3316,162 @@
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>189</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>190</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>191</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>192</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3070,10 +3485,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,84 +3497,94 @@
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>217</v>
-      </c>
-      <c r="B4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>218</v>
-      </c>
-      <c r="B5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>220</v>
-      </c>
-      <c r="B7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>221</v>
-      </c>
-      <c r="B8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>233</v>
-      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Actulizada la planilla de sistemas
Se agregó la pestaña nueva "Tarjetas" con todas las tarjetas cargadas en
el sistema AxTrax, sus respectivos dueños y al área que pertenecen.
</commit_message>
<xml_diff>
--- a/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
+++ b/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="394" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Servidor" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Sistemas" sheetId="6" r:id="rId6"/>
     <sheet name="Usuarios" sheetId="7" r:id="rId7"/>
     <sheet name="Panel de banderas" sheetId="8" r:id="rId8"/>
+    <sheet name="Tarjetas" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="337">
   <si>
     <t>Servidor</t>
   </si>
@@ -867,6 +868,171 @@
   </si>
   <si>
     <t>convenios</t>
+  </si>
+  <si>
+    <t>marce</t>
+  </si>
+  <si>
+    <t>Nombre y apellido</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>Área</t>
+  </si>
+  <si>
+    <t>Número de tarjeta</t>
+  </si>
+  <si>
+    <t>Gabriel Sánchez</t>
+  </si>
+  <si>
+    <t>Germán Kutalek</t>
+  </si>
+  <si>
+    <t>Wilson Gómez</t>
+  </si>
+  <si>
+    <t>Jorge Balcazar</t>
+  </si>
+  <si>
+    <t>Enzo Castillo</t>
+  </si>
+  <si>
+    <t>Manuel Umpierrez</t>
+  </si>
+  <si>
+    <t>Jonatan Soto</t>
+  </si>
+  <si>
+    <t>Adrián Meana</t>
+  </si>
+  <si>
+    <t>Gabriel Zeñiuk</t>
+  </si>
+  <si>
+    <t>Sergio Ochoa</t>
+  </si>
+  <si>
+    <t>Miguel Ángel Riccitelli</t>
+  </si>
+  <si>
+    <t>Sergio Eduardo Gutierre</t>
+  </si>
+  <si>
+    <t>Gustavo Luis Carca</t>
+  </si>
+  <si>
+    <t>Mirta Rojas</t>
+  </si>
+  <si>
+    <t>Llavero 01</t>
+  </si>
+  <si>
+    <t>Llavero 02</t>
+  </si>
+  <si>
+    <t>Randy Speake</t>
+  </si>
+  <si>
+    <t>Pablo Maccari</t>
+  </si>
+  <si>
+    <t>Mantenimiento (master)</t>
+  </si>
+  <si>
+    <t>Bombero 01 (Fernando Sánchez)</t>
+  </si>
+  <si>
+    <t>Mantenimiento</t>
+  </si>
+  <si>
+    <t>CTO</t>
+  </si>
+  <si>
+    <t>Operativa y Logística</t>
+  </si>
+  <si>
+    <t>Limpieza</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>Espacios Físicos</t>
+  </si>
+  <si>
+    <t>Control y Planificación</t>
+  </si>
+  <si>
+    <t>0008382400 | 127,59328</t>
+  </si>
+  <si>
+    <t>0008379433 | 127,56361</t>
+  </si>
+  <si>
+    <t>0008382623 | 127,59551</t>
+  </si>
+  <si>
+    <t>0008383530 | 127,60458</t>
+  </si>
+  <si>
+    <t>0008390124 | 128,01516</t>
+  </si>
+  <si>
+    <t>0008388805 | 128,00197</t>
+  </si>
+  <si>
+    <t>0008384610 | 127,61538</t>
+  </si>
+  <si>
+    <t>0008385792 | 127,62720</t>
+  </si>
+  <si>
+    <t>0008389945 | 128,01337</t>
+  </si>
+  <si>
+    <t>0008389664 | 128,01056</t>
+  </si>
+  <si>
+    <t>0008391207 | 128,02599</t>
+  </si>
+  <si>
+    <t>0008388946 | 128,00338</t>
+  </si>
+  <si>
+    <t>0008386875 | 127,63803</t>
+  </si>
+  <si>
+    <t>0008387294 | 127,64222</t>
+  </si>
+  <si>
+    <t>0008380931 | 127,57859</t>
+  </si>
+  <si>
+    <t>0008383258 | 127,60186</t>
+  </si>
+  <si>
+    <t>0008380357 | 127,57285</t>
+  </si>
+  <si>
+    <t>0008386494 | 127,63422</t>
+  </si>
+  <si>
+    <t>0008385642 | 127,62570</t>
+  </si>
+  <si>
+    <t>0008381101 | 127,58029</t>
+  </si>
+  <si>
+    <t>0008382363 | 127,59291</t>
+  </si>
+  <si>
+    <t>0008380237 | 127,57165</t>
+  </si>
+  <si>
+    <t>0008382231 | 127,59159</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -2182,7 +2348,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,6 +2980,9 @@
       <c r="D19" t="s">
         <v>131</v>
       </c>
+      <c r="F19" t="s">
+        <v>282</v>
+      </c>
       <c r="G19" t="s">
         <v>21</v>
       </c>
@@ -2950,7 +3119,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3588,4 +3757,345 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2">
+        <v>23426675</v>
+      </c>
+      <c r="C2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3">
+        <v>35897670</v>
+      </c>
+      <c r="C3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4">
+        <v>37878033</v>
+      </c>
+      <c r="C4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5">
+        <v>14972197</v>
+      </c>
+      <c r="C5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6">
+        <v>28746454</v>
+      </c>
+      <c r="C6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7">
+        <v>94929982</v>
+      </c>
+      <c r="C7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B8">
+        <v>37900747</v>
+      </c>
+      <c r="C8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9">
+        <v>34932264</v>
+      </c>
+      <c r="C9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10">
+        <v>92821036</v>
+      </c>
+      <c r="C10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B11">
+        <v>32604554</v>
+      </c>
+      <c r="C11" t="s">
+        <v>309</v>
+      </c>
+      <c r="D11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12">
+        <v>29704359</v>
+      </c>
+      <c r="C12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B13">
+        <v>27067242</v>
+      </c>
+      <c r="C13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14">
+        <v>11293948</v>
+      </c>
+      <c r="C14" t="s">
+        <v>311</v>
+      </c>
+      <c r="D14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15">
+        <v>16965144</v>
+      </c>
+      <c r="C15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16">
+        <v>24222400</v>
+      </c>
+      <c r="C16" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17">
+        <v>27257335</v>
+      </c>
+      <c r="C17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B18">
+        <v>20640391</v>
+      </c>
+      <c r="C18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>301</v>
+      </c>
+      <c r="C19" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>302</v>
+      </c>
+      <c r="C20" t="s">
+        <v>312</v>
+      </c>
+      <c r="D20" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>303</v>
+      </c>
+      <c r="C21" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22">
+        <v>23179837</v>
+      </c>
+      <c r="C22" t="s">
+        <v>313</v>
+      </c>
+      <c r="D22" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>305</v>
+      </c>
+      <c r="D23" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>306</v>
+      </c>
+      <c r="B24">
+        <v>32554035</v>
+      </c>
+      <c r="C24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D24" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Carga de planilla de sistemas
Se sube la planilla de sistemas con las tarjetas magnéticas cargadas
actualizadas.
</commit_message>
<xml_diff>
--- a/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
+++ b/3-tecnologia/3-proyecto/Sistemas CCK.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="342">
   <si>
     <t>Servidor</t>
   </si>
@@ -942,6 +942,9 @@
     <t>Mantenimiento (master)</t>
   </si>
   <si>
+    <t>Bombero 01 (Fernando Sánchez)</t>
+  </si>
+  <si>
     <t>Mantenimiento</t>
   </si>
   <si>
@@ -1032,25 +1035,19 @@
     <t>0008382231 | 127,59159</t>
   </si>
   <si>
-    <t>Fernando Sánchez</t>
-  </si>
-  <si>
-    <t>Andrés Habermehl</t>
-  </si>
-  <si>
-    <t>0008380410 | 127,57338</t>
-  </si>
-  <si>
-    <t>Ezequiel Mahafud</t>
-  </si>
-  <si>
-    <t>0008385193 | 127,62121</t>
-  </si>
-  <si>
-    <t>0008380715 | 127,57643</t>
-  </si>
-  <si>
-    <t>0008383067 | 127,59995</t>
+    <t>Marcelo Restuccio</t>
+  </si>
+  <si>
+    <t>0008380735 | 127,57663</t>
+  </si>
+  <si>
+    <t>Mariano Vazquez</t>
+  </si>
+  <si>
+    <t>Zolmaco</t>
+  </si>
+  <si>
+    <t>0008380714 | 127,57642</t>
   </si>
 </sst>
 </file>
@@ -3779,10 +3776,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3814,10 +3811,10 @@
         <v>23426675</v>
       </c>
       <c r="C2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3828,10 +3825,10 @@
         <v>35897670</v>
       </c>
       <c r="C3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3842,10 +3839,10 @@
         <v>37878033</v>
       </c>
       <c r="C4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3856,10 +3853,10 @@
         <v>14972197</v>
       </c>
       <c r="C5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3870,10 +3867,10 @@
         <v>28746454</v>
       </c>
       <c r="C6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3884,10 +3881,10 @@
         <v>94929982</v>
       </c>
       <c r="C7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3898,10 +3895,10 @@
         <v>37900747</v>
       </c>
       <c r="C8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3912,10 +3909,10 @@
         <v>34932264</v>
       </c>
       <c r="C9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3926,10 +3923,10 @@
         <v>92821036</v>
       </c>
       <c r="C10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D10" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3940,10 +3937,10 @@
         <v>32604554</v>
       </c>
       <c r="C11" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D11" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3954,10 +3951,10 @@
         <v>29704359</v>
       </c>
       <c r="C12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3968,10 +3965,10 @@
         <v>27067242</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3982,10 +3979,10 @@
         <v>11293948</v>
       </c>
       <c r="C14" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3996,10 +3993,10 @@
         <v>16965144</v>
       </c>
       <c r="C15" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D15" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4010,10 +4007,10 @@
         <v>24222400</v>
       </c>
       <c r="C16" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D16" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4024,10 +4021,10 @@
         <v>27257335</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D17" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,10 +4035,10 @@
         <v>20640391</v>
       </c>
       <c r="C18" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D18" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4049,10 +4046,10 @@
         <v>301</v>
       </c>
       <c r="C19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D19" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4060,10 +4057,10 @@
         <v>302</v>
       </c>
       <c r="C20" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D20" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4071,10 +4068,10 @@
         <v>303</v>
       </c>
       <c r="C21" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D21" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4085,10 +4082,10 @@
         <v>23179837</v>
       </c>
       <c r="C22" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4096,21 +4093,21 @@
         <v>305</v>
       </c>
       <c r="D23" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
       <c r="B24">
         <v>32554035</v>
       </c>
       <c r="C24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D24" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4118,10 +4115,10 @@
         <v>337</v>
       </c>
       <c r="B25">
-        <v>35970957</v>
+        <v>24946722</v>
       </c>
       <c r="C25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D25" t="s">
         <v>338</v>
@@ -4132,45 +4129,16 @@
         <v>339</v>
       </c>
       <c r="B26">
-        <v>38999220</v>
+        <v>26146963</v>
       </c>
       <c r="C26" t="s">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="D26" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>195</v>
-      </c>
-      <c r="B27">
-        <v>26352654</v>
-      </c>
-      <c r="C27" t="s">
-        <v>312</v>
-      </c>
-      <c r="D27" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B28">
-        <v>33194188</v>
-      </c>
-      <c r="C28" t="s">
-        <v>312</v>
-      </c>
-      <c r="D28" t="s">
-        <v>342</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>